<commit_message>
Now working with data in TestData (example data). Some reworking of gui layout.
</commit_message>
<xml_diff>
--- a/TestData/Schuljahre/SCHULJAHR_2016/Abitur/Ergebnistabellen/K_13/neu/Ergebnisse-01-200301-Stefan_Boellermann.xlsx
+++ b/TestData/Schuljahre/SCHULJAHR_2016/Abitur/Ergebnistabellen/K_13/neu/Ergebnisse-01-200301-Stefan_Boellermann.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Eingabe" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Punktetabelle" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Daten" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Eingabe" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Punktetabelle" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Daten" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.001" refMode="A1"/>

</xml_diff>